<commit_message>
writing the scripts for how to get a complete dataset from all of the excel files I have.
</commit_message>
<xml_diff>
--- a/data/seddataR.xlsx
+++ b/data/seddataR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahferraro/Desktop/Masters/Datasheets/Lab Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1912" documentId="13_ncr:1_{E99D6FA8-A0A2-FD43-B006-A811E6300C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A97BC873-CC09-460C-A515-A1F9AD3943E5}"/>
+  <xr:revisionPtr revIDLastSave="1984" documentId="13_ncr:1_{E99D6FA8-A0A2-FD43-B006-A811E6300C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A84B58B5-9FC3-4629-B1A2-FDF578E9A038}"/>
   <bookViews>
-    <workbookView xWindow="13180" yWindow="500" windowWidth="15240" windowHeight="16440" xr2:uid="{B660C8A4-04E2-6741-A994-6DCDE6E9B9BE}"/>
+    <workbookView xWindow="13180" yWindow="500" windowWidth="15240" windowHeight="16440" activeTab="1" xr2:uid="{B660C8A4-04E2-6741-A994-6DCDE6E9B9BE}"/>
   </bookViews>
   <sheets>
     <sheet name="SEDDATA" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="407">
   <si>
     <t>SAMPLEID</t>
   </si>
@@ -1038,25 +1038,25 @@
     <t>LB-HI-09</t>
   </si>
   <si>
-    <t>570, 571, 572, 573</t>
+    <t>561, 562, 563, 564</t>
   </si>
   <si>
     <t>LB-HO-09</t>
   </si>
   <si>
-    <t>574, 575, 576, 577</t>
+    <t>565, 566, 567, 568</t>
   </si>
   <si>
     <t>LB-SI-09</t>
   </si>
   <si>
-    <t>578, 579, 580, 581</t>
+    <t>569, 570, 571, 572</t>
   </si>
   <si>
     <t>LB-SO-09</t>
   </si>
   <si>
-    <t>582, 583, 584, 585</t>
+    <t>573, 574, 575, 576</t>
   </si>
   <si>
     <t>LB-HI-10</t>
@@ -1201,6 +1201,9 @@
   </si>
   <si>
     <t>141, 142, 143, 144</t>
+  </si>
+  <si>
+    <t>site-treatment-quadrat</t>
   </si>
   <si>
     <t>BB- Brewers Bay</t>
@@ -1662,9 +1665,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AD4D05-27D1-B742-908C-2B53A12F0A39}">
   <dimension ref="A1:U361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F171" sqref="F171"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1"/>
@@ -2497,9 +2500,21 @@
       <c r="F14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="7" t="e">
+      <c r="G14">
+        <v>1.4809504892378391</v>
+      </c>
+      <c r="H14">
+        <v>1.5953333917249846</v>
+      </c>
+      <c r="I14">
+        <v>1.4404918545286827</v>
+      </c>
+      <c r="J14">
+        <v>1.5974101225098392</v>
+      </c>
+      <c r="K14" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.5285464645003364</v>
       </c>
       <c r="R14" s="7">
         <f t="shared" si="1"/>
@@ -2528,9 +2543,21 @@
       <c r="F15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="7" t="e">
+      <c r="G15">
+        <v>1.4898155228409224</v>
+      </c>
+      <c r="H15">
+        <v>1.3333731358820744</v>
+      </c>
+      <c r="I15">
+        <v>1.480033718444862</v>
+      </c>
+      <c r="J15">
+        <v>1.4187272960083839</v>
+      </c>
+      <c r="K15" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.4304874182940608</v>
       </c>
       <c r="R15" s="7">
         <f t="shared" si="1"/>
@@ -2559,9 +2586,21 @@
       <c r="F16" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="K16" s="7" t="e">
+      <c r="G16">
+        <v>1.5079619859416085</v>
+      </c>
+      <c r="H16">
+        <v>1.6184678577470031</v>
+      </c>
+      <c r="I16">
+        <v>1.3855048521384519</v>
+      </c>
+      <c r="J16">
+        <v>1.5116693090529036</v>
+      </c>
+      <c r="K16" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.5059010012199918</v>
       </c>
       <c r="R16" s="7">
         <f t="shared" si="1"/>
@@ -2590,9 +2629,21 @@
       <c r="F17" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="7" t="e">
+      <c r="G17">
+        <v>1.5253876292585036</v>
+      </c>
+      <c r="H17">
+        <v>1.6505443381257132</v>
+      </c>
+      <c r="I17">
+        <v>1.5356383164265446</v>
+      </c>
+      <c r="J17">
+        <v>1.4711966778430909</v>
+      </c>
+      <c r="K17" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.5456917404134631</v>
       </c>
       <c r="R17" s="7">
         <f t="shared" si="1"/>
@@ -2621,9 +2672,21 @@
       <c r="F18" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="K18" s="7" t="e">
+      <c r="G18">
+        <v>1.4436953036163567</v>
+      </c>
+      <c r="H18">
+        <v>1.5566278187230094</v>
+      </c>
+      <c r="I18">
+        <v>1.3996623125521381</v>
+      </c>
+      <c r="J18">
+        <v>1.4568975028602613</v>
+      </c>
+      <c r="K18" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.4642207344379414</v>
       </c>
       <c r="R18" s="7">
         <f t="shared" si="1"/>
@@ -2652,9 +2715,21 @@
       <c r="F19" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="K19" s="7" t="e">
+      <c r="G19">
+        <v>1.4412809072531723</v>
+      </c>
+      <c r="H19">
+        <v>1.54931814625534</v>
+      </c>
+      <c r="I19">
+        <v>1.5082804063315358</v>
+      </c>
+      <c r="J19">
+        <v>1.4700069752873191</v>
+      </c>
+      <c r="K19" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.4922216087818418</v>
       </c>
       <c r="R19" s="7">
         <f t="shared" si="1"/>
@@ -2683,9 +2758,21 @@
       <c r="F20" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="K20" s="7" t="e">
+      <c r="G20">
+        <v>1.4931851803738883</v>
+      </c>
+      <c r="H20">
+        <v>1.5320884539476309</v>
+      </c>
+      <c r="I20">
+        <v>1.4331191978080604</v>
+      </c>
+      <c r="J20">
+        <v>1.326793031011106</v>
+      </c>
+      <c r="K20" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.4462964657851713</v>
       </c>
       <c r="R20" s="7">
         <f t="shared" si="1"/>
@@ -2714,9 +2801,21 @@
       <c r="F21" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="K21" s="7" t="e">
+      <c r="G21">
+        <v>1.4121734345761461</v>
+      </c>
+      <c r="H21">
+        <v>1.5179012509700505</v>
+      </c>
+      <c r="I21">
+        <v>1.469284405940946</v>
+      </c>
+      <c r="J21">
+        <v>1.3942701606743599</v>
+      </c>
+      <c r="K21" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.4484073130403756</v>
       </c>
       <c r="R21" s="7">
         <f t="shared" si="1"/>
@@ -2745,9 +2844,21 @@
       <c r="F22" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="7" t="e">
+      <c r="G22">
+        <v>1.4896895543350168</v>
+      </c>
+      <c r="H22">
+        <v>1.4520687101338929</v>
+      </c>
+      <c r="I22">
+        <v>1.6940209682888501</v>
+      </c>
+      <c r="J22">
+        <v>1.6171539362479077</v>
+      </c>
+      <c r="K22" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.5632332922514169</v>
       </c>
       <c r="R22" s="7">
         <f t="shared" si="1"/>
@@ -2776,9 +2887,21 @@
       <c r="F23" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="K23" s="7" t="e">
+      <c r="G23">
+        <v>1.4466853060690248</v>
+      </c>
+      <c r="H23">
+        <v>1.5975833292054591</v>
+      </c>
+      <c r="I23">
+        <v>1.3605893314079396</v>
+      </c>
+      <c r="J23">
+        <v>1.5123971270870231</v>
+      </c>
+      <c r="K23" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.4793137734423616</v>
       </c>
       <c r="R23" s="7">
         <f t="shared" si="1"/>
@@ -2807,9 +2930,21 @@
       <c r="F24" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K24" s="7" t="e">
+      <c r="G24">
+        <v>1.4283901301488671</v>
+      </c>
+      <c r="H24">
+        <v>1.5073163973488439</v>
+      </c>
+      <c r="I24">
+        <v>1.4282641616429619</v>
+      </c>
+      <c r="J24">
+        <v>1.354945242518351</v>
+      </c>
+      <c r="K24" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.4297289829147559</v>
       </c>
       <c r="R24" s="7">
         <f t="shared" si="1"/>
@@ -2838,9 +2973,21 @@
       <c r="F25" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K25" s="7" t="e">
+      <c r="G25">
+        <v>1.4478190226221721</v>
+      </c>
+      <c r="H25">
+        <v>1.3677327954303176</v>
+      </c>
+      <c r="I25">
+        <v>1.3674546149797764</v>
+      </c>
+      <c r="J25">
+        <v>1.4737038010231225</v>
+      </c>
+      <c r="K25" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.4141775585138472</v>
       </c>
       <c r="R25" s="7">
         <f t="shared" si="1"/>
@@ -8669,9 +8816,27 @@
         <f t="shared" si="4"/>
         <v>1.3851335074804187</v>
       </c>
+      <c r="L146">
+        <v>2.1843973455424583</v>
+      </c>
+      <c r="M146">
+        <v>0.24375893821698336</v>
+      </c>
+      <c r="N146">
+        <v>3.6709218209190144E-3</v>
+      </c>
+      <c r="O146">
+        <v>2.1861025437252075</v>
+      </c>
+      <c r="P146">
+        <v>0.24444101749008307</v>
+      </c>
+      <c r="Q146">
+        <v>3.2493120559162875E-3</v>
+      </c>
       <c r="R146">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>6.9202338768353018</v>
       </c>
       <c r="U146">
         <v>62.5</v>
@@ -8712,9 +8877,27 @@
         <f t="shared" si="4"/>
         <v>1.2611192629792667</v>
       </c>
+      <c r="L147">
+        <v>2.1077679244792189</v>
+      </c>
+      <c r="M147">
+        <v>0.21310716979168765</v>
+      </c>
+      <c r="N147">
+        <v>2.7444922010292391E-3</v>
+      </c>
+      <c r="O147">
+        <v>2.2274129231245738</v>
+      </c>
+      <c r="P147">
+        <v>0.2609651692498296</v>
+      </c>
+      <c r="Q147">
+        <v>3.0689823026803049E-3</v>
+      </c>
       <c r="R147">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.8134745037095437</v>
       </c>
       <c r="U147">
         <v>62.5</v>
@@ -8755,9 +8938,27 @@
         <f t="shared" si="4"/>
         <v>1.2628920072654961</v>
       </c>
+      <c r="L148">
+        <v>1.9710582003877697</v>
+      </c>
+      <c r="M148">
+        <v>0.15842328015510787</v>
+      </c>
+      <c r="N148">
+        <v>1.9711656951799375E-3</v>
+      </c>
+      <c r="O148">
+        <v>2.1284097829919477</v>
+      </c>
+      <c r="P148">
+        <v>0.22136391319677917</v>
+      </c>
+      <c r="Q148">
+        <v>2.6796518993835328E-3</v>
+      </c>
       <c r="R148">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.6508175945634704</v>
       </c>
       <c r="U148">
         <v>12.5</v>
@@ -8798,9 +8999,27 @@
         <f t="shared" si="4"/>
         <v>1.2304481187445619</v>
       </c>
+      <c r="L149">
+        <v>2.1433954551841152</v>
+      </c>
+      <c r="M149">
+        <v>0.22735818207364611</v>
+      </c>
+      <c r="N149">
+        <v>2.9029871877338351E-3</v>
+      </c>
+      <c r="O149">
+        <v>2.0304503908139901</v>
+      </c>
+      <c r="P149">
+        <v>0.18218015632559614</v>
+      </c>
+      <c r="Q149">
+        <v>2.3632522432856513E-3</v>
+      </c>
       <c r="R149">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.2662394310194864</v>
       </c>
       <c r="U149">
         <v>12.5</v>
@@ -8841,9 +9060,27 @@
         <f t="shared" si="4"/>
         <v>1.1731770624035074</v>
       </c>
+      <c r="L150">
+        <v>2.098205767598575</v>
+      </c>
+      <c r="M150">
+        <v>0.20928230703943007</v>
+      </c>
+      <c r="N150">
+        <v>2.3843667298812789E-3</v>
+      </c>
+      <c r="O150">
+        <v>2.1513208381566793</v>
+      </c>
+      <c r="P150">
+        <v>0.2305283352626718</v>
+      </c>
+      <c r="Q150">
+        <v>2.7311874342885348E-3</v>
+      </c>
       <c r="R150">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.1155541641698132</v>
       </c>
       <c r="U150">
         <v>32.5</v>
@@ -8884,9 +9121,27 @@
         <f t="shared" si="4"/>
         <v>1.1487501070240225</v>
       </c>
+      <c r="L151">
+        <v>2.648950354239108</v>
+      </c>
+      <c r="M151">
+        <v>0.42958014169564318</v>
+      </c>
+      <c r="N151">
+        <v>4.6907144431008775E-3</v>
+      </c>
+      <c r="O151">
+        <v>2.2658958058863425</v>
+      </c>
+      <c r="P151">
+        <v>0.27635832235453706</v>
+      </c>
+      <c r="Q151">
+        <v>3.4464755667433992E-3</v>
+      </c>
       <c r="R151">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8.1371900098442769</v>
       </c>
       <c r="U151">
         <v>32.5</v>
@@ -8927,9 +9182,27 @@
         <f t="shared" si="4"/>
         <v>1.173424625508863</v>
       </c>
+      <c r="L152">
+        <v>2.166026884060805</v>
+      </c>
+      <c r="M152">
+        <v>0.23641075362432207</v>
+      </c>
+      <c r="N152">
+        <v>2.8488960747029444E-3</v>
+      </c>
+      <c r="O152">
+        <v>2.1476846379195309</v>
+      </c>
+      <c r="P152">
+        <v>0.22907385516781242</v>
+      </c>
+      <c r="Q152">
+        <v>2.9925970939464535E-3</v>
+      </c>
       <c r="R152">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.8414931686493983</v>
       </c>
       <c r="U152">
         <v>17.5</v>
@@ -8970,9 +9243,27 @@
         <f t="shared" si="4"/>
         <v>1.2899319343612232</v>
       </c>
+      <c r="L153">
+        <v>2.143224069654766</v>
+      </c>
+      <c r="M153">
+        <v>0.22728962786190643</v>
+      </c>
+      <c r="N153">
+        <v>2.7413230595503069E-3</v>
+      </c>
+      <c r="O153">
+        <v>2.1417008276978806</v>
+      </c>
+      <c r="P153">
+        <v>0.22668033107915231</v>
+      </c>
+      <c r="Q153">
+        <v>2.9208006656534472E-3</v>
+      </c>
       <c r="R153">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.6621237252037542</v>
       </c>
       <c r="U153">
         <v>17.5</v>
@@ -9013,9 +9304,27 @@
         <f t="shared" si="4"/>
         <v>1.1575119164347676</v>
       </c>
+      <c r="L154">
+        <v>2.1673054896114365</v>
+      </c>
+      <c r="M154">
+        <v>0.23692219584457463</v>
+      </c>
+      <c r="N154">
+        <v>2.5843385079721594E-3</v>
+      </c>
+      <c r="O154">
+        <v>2.1163190697613401</v>
+      </c>
+      <c r="P154">
+        <v>0.21652762790453606</v>
+      </c>
+      <c r="Q154">
+        <v>2.6328173473459406E-3</v>
+      </c>
       <c r="R154">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.2171558553181008</v>
       </c>
       <c r="U154">
         <v>25</v>
@@ -9056,9 +9365,27 @@
         <f t="shared" si="4"/>
         <v>1.2633713874129686</v>
       </c>
+      <c r="L155">
+        <v>2.3638145554379859</v>
+      </c>
+      <c r="M155">
+        <v>0.31552582217519443</v>
+      </c>
+      <c r="N155">
+        <v>3.6282424920207963E-3</v>
+      </c>
+      <c r="O155">
+        <v>2.397482836056176</v>
+      </c>
+      <c r="P155">
+        <v>0.32899313442247047</v>
+      </c>
+      <c r="Q155">
+        <v>4.80412114251191E-3</v>
+      </c>
       <c r="R155">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8.432363634532706</v>
       </c>
       <c r="U155">
         <v>25</v>
@@ -9099,9 +9426,27 @@
         <f t="shared" si="4"/>
         <v>1.3421646878567126</v>
       </c>
+      <c r="L156">
+        <v>2.1189762060544011</v>
+      </c>
+      <c r="M156">
+        <v>0.21759048242176049</v>
+      </c>
+      <c r="N156">
+        <v>3.1020261020290097E-3</v>
+      </c>
+      <c r="O156">
+        <v>2.0469899512590319</v>
+      </c>
+      <c r="P156">
+        <v>0.18879598050361279</v>
+      </c>
+      <c r="Q156">
+        <v>2.6218221505310982E-3</v>
+      </c>
       <c r="R156">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.7238482525601082</v>
       </c>
       <c r="U156">
         <v>0</v>
@@ -9142,9 +9487,27 @@
         <f t="shared" si="4"/>
         <v>1.3361007039474395</v>
       </c>
+      <c r="L157">
+        <v>2.034345934497745</v>
+      </c>
+      <c r="M157">
+        <v>0.18373837379909808</v>
+      </c>
+      <c r="N157">
+        <v>2.6168885816048146E-3</v>
+      </c>
+      <c r="O157">
+        <v>2.1272412708398649</v>
+      </c>
+      <c r="P157">
+        <v>0.22089650833594598</v>
+      </c>
+      <c r="Q157">
+        <v>2.8684358016406739E-3</v>
+      </c>
       <c r="R157">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.485324383245489</v>
       </c>
       <c r="U157">
         <v>0</v>
@@ -10921,102 +11284,106 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07374C76-7F3C-4CE4-9CE0-8E9D1F397F28}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4"/>
-    <col min="5" max="5" width="10.44140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" style="4" customWidth="1"/>
-    <col min="7" max="17" width="8.88671875" style="4"/>
-    <col min="18" max="18" width="11.109375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="12.5546875" style="4" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="17.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="4"/>
+    <col min="6" max="6" width="10.44140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" style="4" customWidth="1"/>
+    <col min="8" max="18" width="8.88671875" style="4"/>
+    <col min="19" max="19" width="11.109375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" style="4" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="17.25">
+    <row r="1" spans="1:21" ht="36">
       <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="F1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="53.25">
+    <row r="2" spans="1:21" ht="53.25">
       <c r="A2" s="4" t="s">
         <v>387</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>389</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>391</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -11026,76 +11393,79 @@
         <v>393</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>394</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>395</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="Q2" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>396</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>397</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="53.25">
-      <c r="A3" s="4" t="s">
         <v>398</v>
       </c>
+      <c r="U2" s="4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="53.25">
       <c r="B3" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>401</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>402</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="17.25">
-      <c r="A4" s="4" t="s">
         <v>403</v>
       </c>
+      <c r="U3" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="17.25">
       <c r="B4" s="4" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="17.25">
-      <c r="B5" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="17.25">
+      <c r="C5" s="4" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>